<commit_message>
Lots, mostly File stuff
</commit_message>
<xml_diff>
--- a/RunningTheNumbers/Data/Meets Working.xlsx
+++ b/RunningTheNumbers/Data/Meets Working.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vicky Brown\Documents\GitHub\Running-The-Numbers\RunningTheNumbers\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DD9FEC9-2CD6-4AA4-85F1-09713DD1EB12}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02B46070-0AF4-4E9D-846E-E1FE7BFDAC02}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17970" yWindow="1260" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
   <si>
     <t>Name</t>
   </si>
@@ -39,24 +39,6 @@
     <t>Date</t>
   </si>
   <si>
-    <t>Team 1</t>
-  </si>
-  <si>
-    <t>Team 1 Score</t>
-  </si>
-  <si>
-    <t>Team 2</t>
-  </si>
-  <si>
-    <t>Team 2 Score</t>
-  </si>
-  <si>
-    <t>Gender</t>
-  </si>
-  <si>
-    <t>b</t>
-  </si>
-  <si>
     <t>Conditions</t>
   </si>
   <si>
@@ -67,13 +49,70 @@
   </si>
   <si>
     <t>Warm...Mid-80s...Dry &amp; Dusty...Course ran slow</t>
+  </si>
+  <si>
+    <t>Score Set 1</t>
+  </si>
+  <si>
+    <t>Score Set 2</t>
+  </si>
+  <si>
+    <t>Score Set 3</t>
+  </si>
+  <si>
+    <t>Cedar Crest 25 - Annville-Cleona 32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cedar Crest 15 -  Lancaster Catholic 55 </t>
+  </si>
+  <si>
+    <t>Great start ladies...the 2010 CCXC GIRLS are UNDEFEATED!  Be happy with our great start but do not get complacent.  This was a good start for our team, but we have bigger and better competitions on the horizon.  I loved the confident TEAM SWAGGER that you showed before the race today and during the first part of the race.  For the most part you ran smart and strong races and moved up during the race.  If you aren't happy with your time today, don't worry about it.  Saturday you will have the opportunity to cut a HUGE amount of time off of today!  One thing that you really need to focus on improving is getting our post-race routine started shortly after our race is finished.  Other than that, great job and let's keep getting better!!!</t>
+  </si>
+  <si>
+    <t>Cedar Crest 23 - Lancaster Catholic 32</t>
+  </si>
+  <si>
+    <t>Cedar Crest 15 - J.P. McCaskey 52</t>
+  </si>
+  <si>
+    <t>Cedar Crest 15 - Annville-Cleona 52</t>
+  </si>
+  <si>
+    <t>Cedar Crest 20 - J.P. McCaskey 42</t>
+  </si>
+  <si>
+    <t>Overcast &amp; low-70s, but humidity was really high</t>
+  </si>
+  <si>
+    <t>This is a very promising start to our 2010 CCXC season!  We have tremendous depth and we have high quality depth; 12 athletes under 12:00 breaks the old record of 11 athletes in 2008.  I'm also very excited about the 1600 meter times...once you gentlemen develop the endurance to carry your speed for the duration of a 5k, it's going to be exciting!  Whether you had a "GREAT" day or just a "GOOD" day for the time trial, remember that this is only the start of our 2010 XC journey.  There is a lot of hard work to be done!  Commit yourselves to the daily process of becoming a great XC runner &amp; TEAM and be a TEAM on a MISSION in 2010! STUDLY PERFORMANCES: BK, Bryce Ebersole, Devin Gill, Cody Lloyd, Dylan Nixon, Daniel Neiswender, Hunter Adams, Shaun Ditlzer, and I guess Alex Galli</t>
+  </si>
+  <si>
+    <t>I'm really excited for our 2010 season!  I think that we have the potential to rebound strongly from our 10-11 2009 record and make some noise in 2010!  This will only happen, however, if you take it upon yourselves to create an intense work ethic and a positive TEAM attitude.  We will work hard on your endurance for the next several weeks so you  are able to carry your speed for the duration of a 5k...it's going to be exciting!  Whether you had a "GREAT" day or just a "GOOD" day for the time trial, remember that this is only the start of our 2010 XC journey.  There is a lot of hard work to be done!  Commit yourselves to the daily process of becoming a great XC runner &amp; TEAM and be a TEAM on a MISSION in 2010! STUDLY PERFORMANCES: Rebecca Krick, Haley Shiner, Britney Holzman, Kelsey Bachman, Megan Doris, Katrina Diehm, Amanda Kerbis, Erica Bachman, and Haleigh Echard</t>
+  </si>
+  <si>
+    <t>3200 Time Trial (Boys)</t>
+  </si>
+  <si>
+    <t>1600 Time Trial (Boys)</t>
+  </si>
+  <si>
+    <t>3200 Time Trial (Girls)</t>
+  </si>
+  <si>
+    <t>1600 Time Trial (Girls)</t>
+  </si>
+  <si>
+    <t>McCaskey &amp; Annville-Cleona @ Lancaster Catholic (Boys)</t>
+  </si>
+  <si>
+    <t>McCaskey &amp; Annville-Cleona @ Lancaster Catholic (Girls)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -84,6 +123,18 @@
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -109,9 +160,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -392,78 +445,152 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="7.28515625" customWidth="1"/>
+    <col min="1" max="1" width="44.85546875" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" customWidth="1"/>
     <col min="4" max="4" width="10.42578125" customWidth="1"/>
     <col min="5" max="5" width="17.28515625" customWidth="1"/>
-    <col min="6" max="6" width="8.85546875" customWidth="1"/>
-    <col min="7" max="7" width="13" customWidth="1"/>
+    <col min="6" max="6" width="35" customWidth="1"/>
+    <col min="7" max="7" width="33" customWidth="1"/>
+    <col min="8" max="8" width="32.5703125" customWidth="1"/>
     <col min="9" max="9" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
         <v>8</v>
       </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="2">
+        <v>40406</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="2">
+        <v>40406</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="2">
+        <v>40406</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="2">
+        <v>40406</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="2">
+        <v>40428</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" t="s">
         <v>9</v>
       </c>
-      <c r="F1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" t="s">
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="2">
+        <v>40428</v>
+      </c>
+      <c r="C7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="D7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>10</v>
+      <c r="E7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
comments and more meets
</commit_message>
<xml_diff>
--- a/RunningTheNumbers/Data/Meets Working.xlsx
+++ b/RunningTheNumbers/Data/Meets Working.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vicky Brown\Documents\GitHub\Running-The-Numbers\RunningTheNumbers\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02B46070-0AF4-4E9D-846E-E1FE7BFDAC02}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E21FDA50-BB13-4716-89A4-F21FD16FE576}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17940" yWindow="2055" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="59">
   <si>
     <t>Name</t>
   </si>
@@ -106,6 +106,108 @@
   </si>
   <si>
     <t>McCaskey &amp; Annville-Cleona @ Lancaster Catholic (Girls)</t>
+  </si>
+  <si>
+    <t>Elizabethtown &amp; Lebanon &amp; Northern Lebanon @ Hempfield (Boys)</t>
+  </si>
+  <si>
+    <t>Elizabethtown &amp; Lebanon &amp; Northern Lebanon @ Hempfield (Girls)</t>
+  </si>
+  <si>
+    <t>Mid-70s &amp; Clear Skies</t>
+  </si>
+  <si>
+    <t>We had a good race, but we need to step up our game &amp; close that 1:46 gap between #1 &amp; #5 runners in the upcoming races.  Personally, my goal is to have a 60 second spread 1-5 off of Galli &amp; a 20 second gap between #2 &amp; #5.  We can do it...let's get after it!</t>
+  </si>
+  <si>
+    <t>I loved the effort!  Let's get better on Saturday!</t>
+  </si>
+  <si>
+    <t>Cedar Crest 23 - Hempfield 34</t>
+  </si>
+  <si>
+    <t>Cedar Crest 21 - Elizabethtown 37</t>
+  </si>
+  <si>
+    <t>Cedar Crest 15 - Lebanon 55</t>
+  </si>
+  <si>
+    <t>Score Set 4</t>
+  </si>
+  <si>
+    <t>Cedar Crest 15 - Northern Lebanon 55</t>
+  </si>
+  <si>
+    <t>Cedar Crest 36 - Hempfield 19</t>
+  </si>
+  <si>
+    <t>Cedar Crest 32 - Elizabethtown 24</t>
+  </si>
+  <si>
+    <t>Conestoga Valley &amp; Warkwick &amp; Garden Spot &amp; Ephrata @ Home (Boys)</t>
+  </si>
+  <si>
+    <t>Conestoga Valley &amp; Warkwick &amp; Garden Spot &amp; Ephrata @ Home (Girls)</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Lebanon County Meet @ South Hills (Varsity Boys)</t>
+  </si>
+  <si>
+    <t>Mid-60s, Sunny and a Little Breezy</t>
+  </si>
+  <si>
+    <t>Team Results: FIRST PLACE, 28 Points. #1-#5 Spread= 1:20…getting better, but we need to get down to 1:00 or under!</t>
+  </si>
+  <si>
+    <t>Team Results: 1st-9th!</t>
+  </si>
+  <si>
+    <t>Lebanon County Meet @ South Hills (JV Boys)</t>
+  </si>
+  <si>
+    <t>Lebanon County Meet @ South Hills (Varsity Girls)</t>
+  </si>
+  <si>
+    <t>Lebanon County Meet @ South Hills (JV Girls)</t>
+  </si>
+  <si>
+    <t>TEAM Results: 2nd Place, 50 Points</t>
+  </si>
+  <si>
+    <t>Lancaster Mennonite &amp; Columbia &amp; Lampeter-Strasburg @ Donegal (Boys)</t>
+  </si>
+  <si>
+    <t>Lancaster Mennonite &amp; Columbia &amp; Lampeter-Strasburg @ Donegal (Girls)</t>
+  </si>
+  <si>
+    <t>Cedar Crest 15 - Donegal 55</t>
+  </si>
+  <si>
+    <t>Cedar Crest 15 - Columbia 55</t>
+  </si>
+  <si>
+    <t>Cedar Crest 23 - Lancaster Mennonite 34</t>
+  </si>
+  <si>
+    <t>Cedar Crest 17 - Lampeter-Strasburg 44</t>
+  </si>
+  <si>
+    <t>Cedar Crest 15 - Lancaster Mennonite 55</t>
+  </si>
+  <si>
+    <t>Carlisle Meet of Champions (Varsity Boys)</t>
+  </si>
+  <si>
+    <t>Carlisle Meet of Champions (Varsity Girls)</t>
+  </si>
+  <si>
+    <t>Carlisle Meet of Champions (JV Boys)</t>
+  </si>
+  <si>
+    <t>Carlisle Meet of Champions (JV Girls)</t>
   </si>
 </sst>
 </file>
@@ -445,10 +547,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -457,14 +559,14 @@
     <col min="2" max="2" width="14.28515625" customWidth="1"/>
     <col min="3" max="3" width="11.42578125" customWidth="1"/>
     <col min="4" max="4" width="10.42578125" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" customWidth="1"/>
-    <col min="6" max="6" width="35" customWidth="1"/>
+    <col min="5" max="5" width="27.5703125" customWidth="1"/>
+    <col min="6" max="6" width="30.7109375" customWidth="1"/>
     <col min="7" max="7" width="33" customWidth="1"/>
-    <col min="8" max="8" width="32.5703125" customWidth="1"/>
+    <col min="8" max="8" width="33.42578125" customWidth="1"/>
     <col min="9" max="9" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -486,8 +588,11 @@
       <c r="G1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -501,7 +606,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -515,7 +620,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -529,7 +634,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -543,7 +648,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -566,7 +671,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -587,6 +692,250 @@
       </c>
       <c r="G7" s="3" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="2">
+        <v>40435</v>
+      </c>
+      <c r="C8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G8" t="s">
+        <v>32</v>
+      </c>
+      <c r="H8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="2">
+        <v>40435</v>
+      </c>
+      <c r="C9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" t="s">
+        <v>35</v>
+      </c>
+      <c r="F9" t="s">
+        <v>36</v>
+      </c>
+      <c r="G9" t="s">
+        <v>32</v>
+      </c>
+      <c r="H9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" s="2">
+        <v>40439</v>
+      </c>
+      <c r="C10" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" s="2">
+        <v>40439</v>
+      </c>
+      <c r="C11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" s="2">
+        <v>40439</v>
+      </c>
+      <c r="C12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" s="2">
+        <v>40439</v>
+      </c>
+      <c r="C13" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" s="2">
+        <v>40442</v>
+      </c>
+      <c r="C14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" s="2">
+        <v>40442</v>
+      </c>
+      <c r="C15" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>55</v>
+      </c>
+      <c r="B16" s="2">
+        <v>40446</v>
+      </c>
+      <c r="C16" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>57</v>
+      </c>
+      <c r="B17" s="2">
+        <v>40446</v>
+      </c>
+      <c r="C17" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>56</v>
+      </c>
+      <c r="B18" s="2">
+        <v>40446</v>
+      </c>
+      <c r="C18" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>58</v>
+      </c>
+      <c r="B19" s="2">
+        <v>40446</v>
+      </c>
+      <c r="C19" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>48</v>
+      </c>
+      <c r="B20" s="2">
+        <v>40449</v>
+      </c>
+      <c r="C20" t="s">
+        <v>39</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E20" t="s">
+        <v>50</v>
+      </c>
+      <c r="F20" t="s">
+        <v>51</v>
+      </c>
+      <c r="G20" t="s">
+        <v>52</v>
+      </c>
+      <c r="H20" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>49</v>
+      </c>
+      <c r="B21" s="2">
+        <v>40449</v>
+      </c>
+      <c r="C21" t="s">
+        <v>39</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E21" t="s">
+        <v>50</v>
+      </c>
+      <c r="F21" t="s">
+        <v>51</v>
+      </c>
+      <c r="G21" t="s">
+        <v>54</v>
+      </c>
+      <c r="H21" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>